<commit_message>
Ultimos ejemplos de listas enlazadas
</commit_message>
<xml_diff>
--- a/src/Memoria/DibujosLista.xlsx
+++ b/src/Memoria/DibujosLista.xlsx
@@ -466,16 +466,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>366400</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>230325</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>80795</xdr:rowOff>
+      <xdr:rowOff>92134</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>544993</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>408918</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>95677</xdr:rowOff>
+      <xdr:rowOff>107016</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -484,7 +484,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm rot="2034109">
-          <a:off x="3405329" y="2110527"/>
+          <a:off x="990057" y="2121866"/>
           <a:ext cx="938325" cy="1749793"/>
           <a:chOff x="773906" y="2768203"/>
           <a:chExt cx="937617" cy="1756172"/>
@@ -622,30 +622,138 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>647246</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>79829</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>186872</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>134766</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>32023</xdr:rowOff>
+      <xdr:colOff>433614</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>79829</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="40" name="Conector angular 39"/>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="3" idx="6"/>
-          <a:endCxn id="7" idx="7"/>
+          <a:endCxn id="18" idx="2"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5965371" y="1831068"/>
+          <a:ext cx="546100" cy="278493"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>433614</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>595539</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Elipse 17"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="5965371" y="2109561"/>
-          <a:ext cx="247252" cy="1687105"/>
+          <a:off x="6511471" y="1161143"/>
+          <a:ext cx="1681389" cy="1339850"/>
         </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
+        <a:prstGeom prst="ellipse">
           <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-HN" sz="1100"/>
+            <a:t>VICTOR</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>340179</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>4537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>592364</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>113394</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Conector angular 26"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="6189209" y="2070328"/>
+          <a:ext cx="2229304" cy="1771649"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
         </a:prstGeom>
         <a:ln>
           <a:tailEnd type="triangle"/>
@@ -936,8 +1044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>